<commit_message>
Trim and remove equal sign from formulas
This is an advancement toward always-valid model. Equals sign is not a valid part of formula and it's annoying to sometimes have formula with equal sign and sometimes without.
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/Misc/Formulas.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/Misc/Formulas.xlsx
@@ -60,7 +60,7 @@
     <x:t>"Test" &amp; A4 &amp; "R3C2"</x:t>
   </x:si>
   <x:si>
-    <x:t>="Test" &amp; RC[-2] &amp; "R3C2"</x:t>
+    <x:t>"Test" &amp; RC[-2] &amp; "R3C2"</x:t>
   </x:si>
   <x:si>
     <x:t>TestAR3C2</x:t>
@@ -447,7 +447,7 @@
     <x:col min="2" max="2" width="6.139196" style="0" customWidth="1"/>
     <x:col min="3" max="3" width="10.282054" style="0" customWidth="1"/>
     <x:col min="4" max="4" width="19.853482" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="23.996339" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="22.996339" style="0" customWidth="1"/>
     <x:col min="6" max="7" width="10.282054" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>

</xml_diff>